<commit_message>
Update manuals and documents
</commit_message>
<xml_diff>
--- a/afc_saaspro_tax/support_docs/TM_00115_AFC Modules Corresponding Transaction Types.xlsx
+++ b/afc_saaspro_tax/support_docs/TM_00115_AFC Modules Corresponding Transaction Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sanjuan.avalara.com\kc\BillSoft Document Repository\Technical Manuals and Publications_TM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\durcpifsv-wv02\UEMprofiles\Lisa.kelly\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81BA6C8E-0A88-4303-9A0F-892443A3A61A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783D748-A449-4B68-A7D0-A8F3D0DAE28C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="6255" tabRatio="754" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20535" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3172" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="1020">
   <si>
     <t>Local/Centrex Outbound Channel</t>
   </si>
@@ -3083,16 +3083,34 @@
     <t>Timesharing/No Retrieval-Disaster Recovery</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Digital Goods/Streaming Audio</t>
   </si>
   <si>
     <t>Digital Goods/ Downloaded Audio</t>
   </si>
   <si>
-    <t>September 25, 2018</t>
+    <t>April 24, 2019</t>
+  </si>
+  <si>
+    <t>Software/Software Set Up-Optional-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Computer Consulting-Optional-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Computer Training-Optional-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Software Set Up-Mandatory-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Computer Consulting-Mandatory-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Computer Training-Mandatory-Remotely Accessed</t>
+  </si>
+  <si>
+    <t>Software/Modification Charges-Remotely Accessed Software</t>
   </si>
 </sst>
 </file>
@@ -4592,11 +4610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
@@ -4711,7 +4727,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B19" s="8"/>
     </row>
@@ -4729,7 +4745,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="153" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="154" bestFit="1" customWidth="1"/>
@@ -5931,27 +5947,27 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="39" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="28.42578125" bestFit="1" customWidth="1"/>
@@ -7070,18 +7086,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J277"/>
+  <dimension ref="A1:J284"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="116" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" style="116" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
@@ -8396,13 +8410,13 @@
         <v>12</v>
       </c>
       <c r="B75" s="27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C75" s="81">
-        <v>62</v>
+        <v>663</v>
       </c>
       <c r="D75" s="84" t="s">
-        <v>33</v>
+        <v>1013</v>
       </c>
       <c r="E75" s="83" t="s">
         <v>776</v>
@@ -8413,13 +8427,13 @@
         <v>12</v>
       </c>
       <c r="B76" s="27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C76" s="81">
-        <v>646</v>
+        <v>666</v>
       </c>
       <c r="D76" s="84" t="s">
-        <v>31</v>
+        <v>1014</v>
       </c>
       <c r="E76" s="83" t="s">
         <v>776</v>
@@ -8430,13 +8444,13 @@
         <v>12</v>
       </c>
       <c r="B77" s="27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C77" s="81">
-        <v>660</v>
+        <v>667</v>
       </c>
       <c r="D77" s="84" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="E77" s="83" t="s">
         <v>776</v>
@@ -8447,13 +8461,13 @@
         <v>12</v>
       </c>
       <c r="B78" s="27">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C78" s="81">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="D78" s="84" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
       <c r="E78" s="83" t="s">
         <v>776</v>
@@ -8464,13 +8478,13 @@
         <v>12</v>
       </c>
       <c r="B79" s="27">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C79" s="81">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="D79" s="84" t="s">
-        <v>1012</v>
+        <v>1017</v>
       </c>
       <c r="E79" s="83" t="s">
         <v>776</v>
@@ -8481,13 +8495,13 @@
         <v>12</v>
       </c>
       <c r="B80" s="27">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C80" s="81">
-        <v>563</v>
+        <v>670</v>
       </c>
       <c r="D80" s="84" t="s">
-        <v>95</v>
+        <v>1018</v>
       </c>
       <c r="E80" s="83" t="s">
         <v>776</v>
@@ -8498,13 +8512,13 @@
         <v>12</v>
       </c>
       <c r="B81" s="27">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C81" s="81">
-        <v>564</v>
+        <v>671</v>
       </c>
       <c r="D81" s="84" t="s">
-        <v>96</v>
+        <v>1019</v>
       </c>
       <c r="E81" s="83" t="s">
         <v>776</v>
@@ -8515,13 +8529,13 @@
         <v>12</v>
       </c>
       <c r="B82" s="27">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C82" s="81">
-        <v>604</v>
-      </c>
-      <c r="D82" s="85" t="s">
-        <v>97</v>
+        <v>62</v>
+      </c>
+      <c r="D82" s="84" t="s">
+        <v>33</v>
       </c>
       <c r="E82" s="83" t="s">
         <v>776</v>
@@ -8532,13 +8546,13 @@
         <v>12</v>
       </c>
       <c r="B83" s="27">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C83" s="81">
-        <v>605</v>
-      </c>
-      <c r="D83" s="85" t="s">
-        <v>36</v>
+        <v>646</v>
+      </c>
+      <c r="D83" s="84" t="s">
+        <v>31</v>
       </c>
       <c r="E83" s="83" t="s">
         <v>776</v>
@@ -8549,164 +8563,262 @@
         <v>12</v>
       </c>
       <c r="B84" s="27">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C84" s="81">
-        <v>585</v>
+        <v>660</v>
       </c>
       <c r="D84" s="84" t="s">
-        <v>7</v>
+        <v>1009</v>
       </c>
       <c r="E84" s="83" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B85" s="27">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C85" s="81">
-        <v>586</v>
+        <v>661</v>
       </c>
       <c r="D85" s="84" t="s">
-        <v>8</v>
+        <v>1010</v>
       </c>
       <c r="E85" s="83" t="s">
         <v>776</v>
       </c>
-      <c r="F85" s="8"/>
     </row>
     <row r="86" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B86" s="27">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C86" s="81">
-        <v>650</v>
+        <v>662</v>
       </c>
       <c r="D86" s="84" t="s">
-        <v>733</v>
+        <v>1011</v>
       </c>
       <c r="E86" s="83" t="s">
         <v>776</v>
       </c>
-      <c r="F86" s="25"/>
     </row>
     <row r="87" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B87" s="27">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C87" s="81">
-        <v>651</v>
+        <v>563</v>
       </c>
       <c r="D87" s="84" t="s">
-        <v>734</v>
+        <v>95</v>
       </c>
       <c r="E87" s="83" t="s">
         <v>776</v>
       </c>
-      <c r="F87" s="25"/>
     </row>
     <row r="88" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="27">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C88" s="81">
-        <v>652</v>
+        <v>564</v>
       </c>
       <c r="D88" s="84" t="s">
-        <v>735</v>
+        <v>96</v>
       </c>
       <c r="E88" s="83" t="s">
         <v>776</v>
       </c>
-      <c r="F88" s="25"/>
     </row>
     <row r="89" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B89" s="27">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C89" s="81">
-        <v>653</v>
-      </c>
-      <c r="D89" s="84" t="s">
-        <v>738</v>
+        <v>604</v>
+      </c>
+      <c r="D89" s="85" t="s">
+        <v>97</v>
       </c>
       <c r="E89" s="83" t="s">
         <v>776</v>
       </c>
-      <c r="F89" s="25"/>
     </row>
     <row r="90" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B90" s="27">
+        <v>58</v>
+      </c>
+      <c r="C90" s="81">
+        <v>605</v>
+      </c>
+      <c r="D90" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90" s="83" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="27">
+        <v>61</v>
+      </c>
+      <c r="C91" s="81">
+        <v>585</v>
+      </c>
+      <c r="D91" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="83" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="27">
+        <v>61</v>
+      </c>
+      <c r="C92" s="81">
+        <v>586</v>
+      </c>
+      <c r="D92" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="27">
+        <v>61</v>
+      </c>
+      <c r="C93" s="81">
+        <v>650</v>
+      </c>
+      <c r="D93" s="84" t="s">
+        <v>733</v>
+      </c>
+      <c r="E93" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="F93" s="25"/>
+    </row>
+    <row r="94" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="27">
+        <v>61</v>
+      </c>
+      <c r="C94" s="81">
+        <v>651</v>
+      </c>
+      <c r="D94" s="84" t="s">
+        <v>734</v>
+      </c>
+      <c r="E94" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="F94" s="25"/>
+    </row>
+    <row r="95" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="27">
+        <v>61</v>
+      </c>
+      <c r="C95" s="81">
+        <v>652</v>
+      </c>
+      <c r="D95" s="84" t="s">
+        <v>735</v>
+      </c>
+      <c r="E95" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="F95" s="25"/>
+    </row>
+    <row r="96" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="27">
+        <v>61</v>
+      </c>
+      <c r="C96" s="81">
+        <v>653</v>
+      </c>
+      <c r="D96" s="84" t="s">
+        <v>738</v>
+      </c>
+      <c r="E96" s="83" t="s">
+        <v>776</v>
+      </c>
+      <c r="F96" s="25"/>
+    </row>
+    <row r="97" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="27">
         <v>64</v>
       </c>
-      <c r="C90" s="81">
+      <c r="C97" s="81">
         <v>648</v>
       </c>
-      <c r="D90" s="84" t="s">
+      <c r="D97" s="84" t="s">
         <v>736</v>
       </c>
-      <c r="E90" s="83" t="s">
+      <c r="E97" s="83" t="s">
         <v>777</v>
       </c>
-      <c r="F90" s="25"/>
-    </row>
-    <row r="91" spans="1:6" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="66" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B91" s="67">
+      <c r="F97" s="25"/>
+    </row>
+    <row r="98" spans="1:6" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="67">
         <v>64</v>
       </c>
-      <c r="C91" s="82">
+      <c r="C98" s="82">
         <v>649</v>
       </c>
-      <c r="D91" s="86" t="s">
+      <c r="D98" s="86" t="s">
         <v>737</v>
       </c>
-      <c r="E91" s="120" t="s">
+      <c r="E98" s="120" t="s">
         <v>777</v>
       </c>
-      <c r="F91" s="25"/>
-    </row>
-    <row r="255" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D255" s="24"/>
-    </row>
-    <row r="256" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D256" s="24"/>
-    </row>
-    <row r="257" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D257" s="24"/>
-    </row>
-    <row r="258" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D258" s="24"/>
-    </row>
-    <row r="259" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D259" s="24"/>
-    </row>
-    <row r="260" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D260" s="24"/>
-    </row>
-    <row r="261" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D261" s="24"/>
+      <c r="F98" s="25"/>
     </row>
     <row r="262" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D262" s="24"/>
@@ -8756,9 +8868,30 @@
     <row r="277" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D277" s="24"/>
     </row>
+    <row r="278" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D278" s="24"/>
+    </row>
+    <row r="279" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D279" s="24"/>
+    </row>
+    <row r="280" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D280" s="24"/>
+    </row>
+    <row r="281" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D281" s="24"/>
+    </row>
+    <row r="282" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D282" s="24"/>
+    </row>
+    <row r="283" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D283" s="24"/>
+    </row>
+    <row r="284" spans="4:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D284" s="24"/>
+    </row>
   </sheetData>
-  <sortState ref="A13:D235">
-    <sortCondition ref="A13:A235" customList="CORE,Cable &amp; Satellite TV,Local,Long-Distance,International,VoIP,Wireless"/>
+  <sortState ref="A13:D242">
+    <sortCondition ref="A13:A242" customList="CORE,Cable &amp; Satellite TV,Local,Long-Distance,International,VoIP,Wireless"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="C3:C4"/>
@@ -8776,17 +8909,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.28515625" style="129" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9177,7 +9308,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -9390,9 +9521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -10111,7 +10242,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -10562,7 +10693,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -11970,7 +12101,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -12459,12 +12590,12 @@
       <selection activeCell="J468" sqref="J468"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="79" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="79" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>

</xml_diff>